<commit_message>
Guarda todos los pdf
</commit_message>
<xml_diff>
--- a/GestionHotel/trabajadoresLIKEATHOME.xlsx
+++ b/GestionHotel/trabajadoresLIKEATHOME.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Nominas_2016_Grupo1\B\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1545" yWindow="1320" windowWidth="19440" windowHeight="15375"/>
   </bookViews>
@@ -158,24 +163,15 @@
     <t>Cocinero</t>
   </si>
   <si>
-    <t>Cuidador</t>
-  </si>
-  <si>
     <t>Ordenanza</t>
   </si>
   <si>
     <t>Calefactor</t>
   </si>
   <si>
-    <t>Jefe división</t>
-  </si>
-  <si>
     <t>Coordinador</t>
   </si>
   <si>
-    <t>Jefe de servicio</t>
-  </si>
-  <si>
     <t>Jefe de sección</t>
   </si>
   <si>
@@ -276,6 +272,15 @@
   </si>
   <si>
     <t>Marín</t>
+  </si>
+  <si>
+    <t>Jefe del hotel</t>
+  </si>
+  <si>
+    <t>Conserje</t>
+  </si>
+  <si>
+    <t>Secretario</t>
   </si>
 </sst>
 </file>
@@ -392,7 +397,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,7 +432,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -638,7 +643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -699,7 +706,7 @@
         <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -707,25 +714,25 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1">
         <v>40299</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I2" s="4">
         <v>1.8265301202015601E+18</v>
@@ -751,7 +758,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1">
         <v>42491</v>
@@ -760,10 +767,10 @@
         <v>43</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I3" s="4">
         <v>2.0960043013000102E+19</v>
@@ -774,7 +781,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
@@ -783,7 +790,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E4" s="1">
         <v>39203</v>
@@ -792,10 +799,10 @@
         <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I4" s="4">
         <v>2.0960043013096198E+19</v>
@@ -815,25 +822,25 @@
         <v>38</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1">
         <v>40299</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I5" s="4">
         <v>2.0960056163231498E+19</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -847,7 +854,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E6" s="1">
         <v>42491</v>
@@ -856,74 +863,74 @@
         <v>43</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I6" s="4">
         <v>2.0960043083071402E+19</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E7" s="1">
         <v>39203</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I7" s="4">
         <v>2.0960043073468899E+19</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E8" s="1">
         <v>40299</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I8" s="4">
         <v>2.0960043022159E+19</v>
@@ -940,16 +947,16 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E9" s="1">
         <v>42491</v>
@@ -958,10 +965,10 @@
         <v>43</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I9" s="4">
         <v>2.0960043013000102E+19</v>
@@ -975,16 +982,16 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1">
         <v>39203</v>
@@ -993,16 +1000,16 @@
         <v>13</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I10" s="4">
         <v>2.0960043013000102E+19</v>
       </c>
       <c r="K10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="L10" s="1">
         <v>42459</v>
@@ -1024,7 +1031,7 @@
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1149,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>18000</v>
@@ -1168,7 +1175,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="B6" s="2">
         <v>25000</v>
@@ -1246,7 +1253,7 @@
     </row>
     <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B9">
         <v>30000</v>
@@ -1324,7 +1331,7 @@
     </row>
     <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="B12" s="2">
         <v>20000</v>
@@ -1344,7 +1351,7 @@
     </row>
     <row r="13" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>16000</v>
@@ -1364,7 +1371,7 @@
     </row>
     <row r="14" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2">
         <v>10500</v>
@@ -1384,7 +1391,7 @@
     </row>
     <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>30000</v>
@@ -1420,7 +1427,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B18">
         <v>4.7</v>
@@ -1440,7 +1447,7 @@
     </row>
     <row r="19" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19">
         <v>1.6</v>
@@ -1460,7 +1467,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B20">
         <v>0.1</v>
@@ -1480,7 +1487,7 @@
     </row>
     <row r="21" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>23.6</v>
@@ -1500,7 +1507,7 @@
     </row>
     <row r="22" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>0.2</v>
@@ -1520,7 +1527,7 @@
     </row>
     <row r="23" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B23">
         <v>6.7</v>
@@ -1540,7 +1547,7 @@
     </row>
     <row r="24" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B24">
         <v>0.6</v>
@@ -1560,7 +1567,7 @@
     </row>
     <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1578,7 +1585,7 @@
         <v>18.63</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>8</v>
       </c>
@@ -1592,7 +1599,7 @@
         <v>18.940000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>9</v>
       </c>
@@ -1606,7 +1613,7 @@
         <v>19.25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>10</v>
       </c>
@@ -1620,7 +1627,7 @@
         <v>19.559999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>11</v>
       </c>
@@ -1634,7 +1641,7 @@
         <v>19.87</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>12</v>
       </c>
@@ -1648,7 +1655,7 @@
         <v>20.18</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>13</v>
       </c>
@@ -1662,7 +1669,7 @@
         <v>20.49</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>14</v>
       </c>
@@ -1676,7 +1683,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="33" spans="4:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>15</v>
       </c>
@@ -1690,7 +1697,7 @@
         <v>21.11</v>
       </c>
     </row>
-    <row r="34" spans="4:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>16</v>
       </c>
@@ -1704,7 +1711,7 @@
         <v>21.42</v>
       </c>
     </row>
-    <row r="35" spans="4:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>17</v>
       </c>
@@ -1718,7 +1725,7 @@
         <v>21.72</v>
       </c>
     </row>
-    <row r="36" spans="4:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>18</v>
       </c>
@@ -1732,7 +1739,7 @@
         <v>22.02</v>
       </c>
     </row>
-    <row r="37" spans="4:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F37">
         <v>47000</v>
       </c>
@@ -1740,7 +1747,7 @@
         <v>22.32</v>
       </c>
     </row>
-    <row r="38" spans="4:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F38">
         <v>48000</v>
       </c>
@@ -1748,7 +1755,7 @@
         <v>22.62</v>
       </c>
     </row>
-    <row r="39" spans="4:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
       <c r="F39">
         <v>49000</v>
       </c>

</xml_diff>